<commit_message>
Seleção de dias de antecedência para aviso
</commit_message>
<xml_diff>
--- a/Planilha Datas VPN.xlsx
+++ b/Planilha Datas VPN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Python\DatasVPN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE2F427-E923-44B7-A84A-51FF7501A176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5393DA12-5702-4858-B97B-FDC0DF91FD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -716,7 +716,7 @@
   <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>45221</v>
+        <v>45284</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>45226</v>
+        <v>45285</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>45226</v>
+        <v>45286</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>45239</v>
+        <v>45287</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>45279</v>
+        <v>45288</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>45279</v>
+        <v>45289</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>1</v>
@@ -791,7 +791,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>45284</v>
+        <v>45290</v>
       </c>
       <c r="E8" s="4"/>
     </row>
@@ -800,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>45284</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2">
-        <v>45298</v>
+        <v>45292</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>